<commit_message>
All CRUD and Updated data sets
</commit_message>
<xml_diff>
--- a/attendance/src/main/resources/CRUDOperations.xlsx
+++ b/attendance/src/main/resources/CRUDOperations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="96">
   <si>
     <t xml:space="preserve">TCID</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">User can create policy with Same Name</t>
   </si>
   <si>
-    <t xml:space="preserve">com.darwinbox.attendance.policies.CreatePolicyWithSameName</t>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.policies.CreatePolicyWithSameName</t>
   </si>
   <si>
     <t xml:space="preserve">CRUD.xlsx</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">User can create policy with Same Name in Different Companies</t>
   </si>
   <si>
-    <t xml:space="preserve">com.darwinbox.attendance.policies.CreatePolicyWithSameNameInDiffCompanies</t>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.policies.CreatePolicyWithSameNameInDiffCompanies</t>
   </si>
   <si>
     <t xml:space="preserve">3</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">User can update existing policy with Same Name</t>
   </si>
   <si>
-    <t xml:space="preserve">com.darwinbox.attendance.policies.UpdateExistingPolicyWithSameName</t>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.policies.UpdateExistingPolicyWithSameName</t>
   </si>
   <si>
     <t xml:space="preserve">4,5</t>
@@ -94,238 +94,220 @@
     <t xml:space="preserve">4</t>
   </si>
   <si>
-    <t xml:space="preserve">User can update existing policy with Different Companies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.policies.CreatePolicyWithExistingNameInDiffCompanies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,7,8,9</t>
+    <t xml:space="preserve">User can delete attendance policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.policies.DeleteAttendancePolicy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6,7</t>
   </si>
   <si>
     <t xml:space="preserve">5</t>
   </si>
   <si>
-    <t xml:space="preserve">User can delete attendance policy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.policies.DeleteAttendancePolicy</t>
+    <t xml:space="preserve">Shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can create Shift with Same Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.shifts.CreateShiftWithSameName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shifts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can create Shift with Same Name in Different Companies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.shifts.CreateShiftWithSameNameInDiffCompanies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can update existing Shift with Same Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.shifts.CreateShiftWithExistingName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can delete attendance Shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.shifts.DeleteAttendanceShift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPRestrictions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can create IPRestrictions with Same Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.iprestrictions.CreateIPRestrictionWithSameName</t>
   </si>
   <si>
     <t xml:space="preserve">all</t>
   </si>
   <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can create Shift with Same Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.shifts.CreateShiftWithSameName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shifts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can create Shift with Same Name in Different Companies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.shifts.CreateShiftWithSameNameInDiffCompanies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can update existing Shift with Same Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.shifts.CreateShiftWithExistingName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can update existing Shift with Different Companies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.shifts.CreateShiftWithExistingNameInDiffCompanies</t>
-  </si>
-  <si>
     <t xml:space="preserve">10</t>
   </si>
   <si>
-    <t xml:space="preserve">User can delete attendance Shift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.shifts.DeleteAttendanceShift</t>
+    <t xml:space="preserve">User can create IPRestrictions with Same Name in Different Companies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.iprestrictions.CreateIPRestrictionWithSameNameInDiffCompanies</t>
   </si>
   <si>
     <t xml:space="preserve">11</t>
   </si>
   <si>
-    <t xml:space="preserve">IPRestrictions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can create IPRestrictions with Same Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.iprestrictions.CreateIPRestrictionWithSameName</t>
+    <t xml:space="preserve">User can update existing IPRestrictions with Same Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.iprestrictions.CreateIPRestrictionWithExistingName</t>
   </si>
   <si>
     <t xml:space="preserve">12</t>
   </si>
   <si>
-    <t xml:space="preserve">User can create IPRestrictions with Same Name in Different Companies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.iprestrictions.CreateIPRestrictionWithSameNameInDiffCompanies</t>
+    <t xml:space="preserve">User can update existing IPRestrictions with Different Companies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.iprestrictions.CreateIPRestrictionWithExistingNameInDiffCompanies</t>
   </si>
   <si>
     <t xml:space="preserve">13</t>
   </si>
   <si>
-    <t xml:space="preserve">User can update existing IPRestrictions with Same Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.iprestrictions.CreateIPRestrictionWithExistingName</t>
+    <t xml:space="preserve">User can delete attendance IPRestrictions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.iprestrictions.DeleteAttendanceIPRestriction</t>
   </si>
   <si>
     <t xml:space="preserve">14</t>
   </si>
   <si>
-    <t xml:space="preserve">User can update existing IPRestrictions with Different Companies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.iprestrictions.CreateIPRestrictionWithExistingNameInDiffCompanies</t>
+    <t xml:space="preserve">GeoFencing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can create GeoFencing with Same Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.geofencing.CreateGeoFencingWithSameName</t>
   </si>
   <si>
     <t xml:space="preserve">15</t>
   </si>
   <si>
-    <t xml:space="preserve">User can delete attendance IPRestrictions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.iprestrictions.DeleteAttendanceIPRestriction</t>
+    <t xml:space="preserve">User can create GeoFencing with Same Name in Different Companies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.geofencing.CreateGeoFencingWithSameNameInDiffCompanies</t>
   </si>
   <si>
     <t xml:space="preserve">16</t>
   </si>
   <si>
-    <t xml:space="preserve">GeoFencing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can create GeoFencing with Same Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.geofencing.CreateGeoFencingWithSameName</t>
+    <t xml:space="preserve">User can update existing GeoFencing with Same Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.geofencing.CreateGeoFencingWithExistingName</t>
   </si>
   <si>
     <t xml:space="preserve">17</t>
   </si>
   <si>
-    <t xml:space="preserve">User can create GeoFencing with Same Name in Different Companies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.geofencing.CreateGeoFencingWithSameNameInDiffCompanies</t>
+    <t xml:space="preserve">User can update existing GeoFencing with Different Companies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.geofencing.CreateGeoFencingWithExistingNameInDiffCompanies</t>
   </si>
   <si>
     <t xml:space="preserve">18</t>
   </si>
   <si>
-    <t xml:space="preserve">User can update existing GeoFencing with Same Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.geofencing.CreateGeoFencingWithExistingName</t>
+    <t xml:space="preserve">User can delete attendance GeoFencing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.geofencing.DeleteAttendanceGeoFencing</t>
   </si>
   <si>
     <t xml:space="preserve">19</t>
   </si>
   <si>
-    <t xml:space="preserve">User can update existing GeoFencing with Different Companies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.geofencing.CreateGeoFencingWithExistingNameInDiffCompanies</t>
+    <t xml:space="preserve">WeeklyOff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can create WeeklyOff with Same Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.weeklyoff.CreateWeeklyoffWithSameName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weeklyoff</t>
   </si>
   <si>
     <t xml:space="preserve">20</t>
   </si>
   <si>
-    <t xml:space="preserve">User can delete attendance GeoFencing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.geofencing.DeleteAttendanceGeoFencing</t>
+    <t xml:space="preserve">User can update existing WeeklyOff with Same Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.weeklyoff.CreateWeeklyoffWithExistingName</t>
   </si>
   <si>
     <t xml:space="preserve">21</t>
   </si>
   <si>
-    <t xml:space="preserve">WeeklyOff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can create WeeklyOff with Same Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.weeklyoff.CreateWeeklyoffWithSameName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weeklyoff</t>
+    <t xml:space="preserve">User can delete attendance WeeklyOff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.weeklyoff.DeleteAttendanceWeeklyoff</t>
   </si>
   <si>
     <t xml:space="preserve">22</t>
   </si>
   <si>
-    <t xml:space="preserve">User can update existing WeeklyOff with Same Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.weeklyoff.CreateWeeklyoffWithExistingName</t>
+    <t xml:space="preserve">Regularisations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can create Attendance Regularisation Reason with Same Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.regreason.CreateRegReasonWithSameName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RegReason</t>
   </si>
   <si>
     <t xml:space="preserve">23</t>
   </si>
   <si>
-    <t xml:space="preserve">User can delete attendance WeeklyOff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.weeklyoff.DeleteAttendanceWeeklyoff</t>
+    <t xml:space="preserve">User can update existing Attendance Regularisation Reason with Same Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.regreason.CreateRegReasonWithExistingName</t>
   </si>
   <si>
     <t xml:space="preserve">24</t>
   </si>
   <si>
-    <t xml:space="preserve">Regularisations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can create Attendance Regularisation Reason with Same Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.regreason.CreateRegReasonWithSameName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RegReason</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can update existing Attendance Regularisation Reason with Same Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.regreason.CreateRegReasonWithExistingName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
     <t xml:space="preserve">User can delete attendance Attendance Regularisation Reason</t>
   </si>
   <si>
-    <t xml:space="preserve">com.darwinbox.attendance.regreason.DeleteAttendanceRegReason</t>
+    <t xml:space="preserve">com.darwinbox.attendance.crud.regreason.DeleteAttendanceRegReason</t>
   </si>
 </sst>
 </file>
@@ -442,10 +424,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -597,33 +579,33 @@
         <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>33</v>
@@ -635,73 +617,73 @@
         <v>13</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="F8" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="F9" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>43</v>
@@ -713,62 +695,62 @@
         <v>13</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="0" t="s">
         <v>51</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -779,7 +761,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>53</v>
@@ -791,13 +773,13 @@
         <v>13</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -805,25 +787,25 @@
         <v>9</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>58</v>
       </c>
@@ -831,74 +813,74 @@
         <v>9</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D15" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="H15" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="0" t="s">
         <v>67</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -909,7 +891,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>69</v>
@@ -921,10 +903,10 @@
         <v>13</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -935,22 +917,22 @@
         <v>9</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -961,74 +943,74 @@
         <v>9</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D21" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="H21" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1039,128 +1021,78 @@
         <v>9</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="0" t="s">
         <v>87</v>
       </c>
+      <c r="E23" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="F23" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D24" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>84</v>
-      </c>
       <c r="H24" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1393,8 +1325,6 @@
     <row r="257" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="258" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="259" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="260" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="261" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>